<commit_message>
feat: add data in manufacturing_materal.xlsx
</commit_message>
<xml_diff>
--- a/DATA/TABLE/MANUFACTURING_MATERIAL.xlsx
+++ b/DATA/TABLE/MANUFACTURING_MATERIAL.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pat/Desktop/St.Gabriel/text2sql/stgabriel-text2sql-main/DATA/TABLE/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tanyatonoran/Documents/Royal-Can-Text2SQL/DATA/TABLE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4AC559C9-F830-494C-AFFD-7F9E53A7818C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E21A6CF7-3A03-FC47-9B53-10ECC649D154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3500" yWindow="3820" windowWidth="25640" windowHeight="14440" xr2:uid="{4F6054FA-D499-CD46-8DC5-11C5F98F5961}"/>
   </bookViews>
@@ -33,6 +33,188 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="59">
+  <si>
+    <t>SalesOrder</t>
+  </si>
+  <si>
+    <t>MG2</t>
+  </si>
+  <si>
+    <t>Material1</t>
+  </si>
+  <si>
+    <t>MaterialDes</t>
+  </si>
+  <si>
+    <t>Uom</t>
+  </si>
+  <si>
+    <t>MatGroup1</t>
+  </si>
+  <si>
+    <t>MatGroup3</t>
+  </si>
+  <si>
+    <t>MatGroup4</t>
+  </si>
+  <si>
+    <t>PricingUnit</t>
+  </si>
+  <si>
+    <t>NetPrice</t>
+  </si>
+  <si>
+    <t>SO2000</t>
+  </si>
+  <si>
+    <t>END</t>
+  </si>
+  <si>
+    <t>MAT101</t>
+  </si>
+  <si>
+    <t>Plastic</t>
+  </si>
+  <si>
+    <t>SHT</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Size1</t>
+  </si>
+  <si>
+    <t>Z01</t>
+  </si>
+  <si>
+    <t>SO2001</t>
+  </si>
+  <si>
+    <t>MAT102</t>
+  </si>
+  <si>
+    <t>Recycled Plastic</t>
+  </si>
+  <si>
+    <t>PCS</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Size2</t>
+  </si>
+  <si>
+    <t>SO2002</t>
+  </si>
+  <si>
+    <t>SOT</t>
+  </si>
+  <si>
+    <t>MAT103</t>
+  </si>
+  <si>
+    <t>Aluminum</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Size3</t>
+  </si>
+  <si>
+    <t>999</t>
+  </si>
+  <si>
+    <t>SO2003</t>
+  </si>
+  <si>
+    <t>POE</t>
+  </si>
+  <si>
+    <t>MAT104</t>
+  </si>
+  <si>
+    <t>Steel</t>
+  </si>
+  <si>
+    <t>Size4</t>
+  </si>
+  <si>
+    <t>SO2004</t>
+  </si>
+  <si>
+    <t>MAT105</t>
+  </si>
+  <si>
+    <t>Alloy</t>
+  </si>
+  <si>
+    <t>Size5</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>SO2005</t>
+  </si>
+  <si>
+    <t>2PC</t>
+  </si>
+  <si>
+    <t>Size6</t>
+  </si>
+  <si>
+    <t>OEM</t>
+  </si>
+  <si>
+    <t>SO2006</t>
+  </si>
+  <si>
+    <t>EOE</t>
+  </si>
+  <si>
+    <t>BLK</t>
+  </si>
+  <si>
+    <t>Size7</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>SO2007</t>
+  </si>
+  <si>
+    <t>Size8</t>
+  </si>
+  <si>
+    <t>SO2008</t>
+  </si>
+  <si>
+    <t>EOS</t>
+  </si>
+  <si>
+    <t>SH</t>
+  </si>
+  <si>
+    <t>Size9</t>
+  </si>
+  <si>
+    <t>SO2009</t>
+  </si>
+  <si>
+    <t>Size10</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -66,8 +248,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,12 +587,367 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B77A01C-D9D9-4F4F-87E7-3347FF3FFCF0}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:J11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2">
+        <v>8</v>
+      </c>
+      <c r="J2">
+        <v>83.57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3">
+        <v>8</v>
+      </c>
+      <c r="J3">
+        <v>47.63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="J4">
+        <v>18.309999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5">
+        <v>8</v>
+      </c>
+      <c r="J5">
+        <v>23.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6">
+        <v>2</v>
+      </c>
+      <c r="J6">
+        <v>37.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" t="s">
+        <v>45</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <v>12.87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" t="s">
+        <v>49</v>
+      </c>
+      <c r="H8" t="s">
+        <v>50</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>46.68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" t="s">
+        <v>52</v>
+      </c>
+      <c r="H9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9">
+        <v>10</v>
+      </c>
+      <c r="J9">
+        <v>97.57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" t="s">
+        <v>56</v>
+      </c>
+      <c r="H10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I10">
+        <v>4</v>
+      </c>
+      <c r="J10">
+        <v>32.31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H11" t="s">
+        <v>41</v>
+      </c>
+      <c r="I11">
+        <v>4</v>
+      </c>
+      <c r="J11">
+        <v>60.73</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>